<commit_message>
update read file excel
</commit_message>
<xml_diff>
--- a/temp/test.xlsx
+++ b/temp/test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D82505-A914-4D29-9D84-EAF85CA9A8A6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B16A76-E9BE-45A0-9ECC-C9DA7D7B42DB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>STT</t>
   </si>
@@ -170,24 +170,6 @@
   </si>
   <si>
     <t>hovaten20</t>
-  </si>
-  <si>
-    <t>Chú thích</t>
-  </si>
-  <si>
-    <t>điểm số được chia đều cho các câu</t>
-  </si>
-  <si>
-    <t>1 câu có thể có nhiều G, 1 G có thể thuộc nhiều câu</t>
-  </si>
-  <si>
-    <t>ví dụ câu 1: G1, G3</t>
-  </si>
-  <si>
-    <t>câu 2: G2,G3</t>
-  </si>
-  <si>
-    <t>Yêu cầu: từ số điểm và tổng điểm tính ra mỗi G đạt bao nhiêu %</t>
   </si>
 </sst>
 </file>
@@ -530,7 +512,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="D3" sqref="D3:H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -544,7 +526,7 @@
     <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -569,11 +551,9 @@
       <c r="H1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -598,11 +578,8 @@
       <c r="H2" s="3">
         <v>10</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -627,11 +604,8 @@
       <c r="H3" s="3">
         <v>10</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -656,11 +630,8 @@
       <c r="H4" s="3">
         <v>10</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -685,11 +656,8 @@
       <c r="H5" s="3">
         <v>10</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -715,7 +683,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -741,7 +709,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -766,11 +734,8 @@
       <c r="H8" s="3">
         <v>10</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -796,7 +761,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -822,7 +787,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -848,7 +813,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -874,7 +839,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -885,7 +850,7 @@
         <v>39</v>
       </c>
       <c r="D13" s="3">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="E13" s="3">
         <v>2</v>
@@ -900,7 +865,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -926,7 +891,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -952,7 +917,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -978,7 +943,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1004,7 +969,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -1030,7 +995,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -1056,7 +1021,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -1082,7 +1047,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>20</v>
       </c>

</xml_diff>